<commit_message>
add score to gn sample
</commit_message>
<xml_diff>
--- a/New_Dataset/model_evaluation_results_gn.xlsx
+++ b/New_Dataset/model_evaluation_results_gn.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Firesoft\Documents\Computing\VetHelper\New_Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\VetHelper\New_Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CCF066-E9E5-4C83-BBEA-7F328B4D186F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6E95F3-A8A4-45F2-A143-EC90AB498002}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>interpretation and recommendation</t>
   </si>
@@ -233,6 +240,9 @@
 -	 ยาต้านจุลชีพที่แนะนำ ได้แก่
      o 	Sulfamethoxazole/trimethoprim 30 mg/kg q12h PO AC for 10-14 days หรือให้ยาต่อเนื่องจนอาการหายสนิท และให้ยา
         ต่อไปอีก 1-2 สัปดาห์</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
@@ -261,7 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -284,13 +294,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -595,15 +619,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,8 +664,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -678,8 +705,11 @@
       <c r="L2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -716,8 +746,11 @@
       <c r="L3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -754,8 +787,11 @@
       <c r="L4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -792,8 +828,11 @@
       <c r="L5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -830,8 +869,11 @@
       <c r="L6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -868,8 +910,11 @@
       <c r="L7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -906,8 +951,11 @@
       <c r="L8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -944,8 +992,11 @@
       <c r="L9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -982,8 +1033,11 @@
       <c r="L10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1020,8 +1074,11 @@
       <c r="L11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1058,8 +1115,11 @@
       <c r="L12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1096,8 +1156,11 @@
       <c r="L13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1134,8 +1197,11 @@
       <c r="L14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1172,8 +1238,11 @@
       <c r="L15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1210,8 +1279,11 @@
       <c r="L16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1248,8 +1320,11 @@
       <c r="L17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1286,8 +1361,11 @@
       <c r="L18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1324,8 +1402,11 @@
       <c r="L19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1362,8 +1443,11 @@
       <c r="L20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1399,6 +1483,9 @@
       </c>
       <c r="L21" t="b">
         <v>0</v>
+      </c>
+      <c r="M21">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>